<commit_message>
:earth_africa: Biogeographic data tables
</commit_message>
<xml_diff>
--- a/input_data/Biogeographic_data/Ponerinae_Biogeography_Genera_summary.xlsx
+++ b/input_data/Biogeographic_data/Ponerinae_Biogeography_Genera_summary.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mael_D\R_projects\Ponerinae_Historical_Biogeography\input_data\Biogeographic_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5B81E40-BC4A-4238-9366-E8B340679C23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87C57E0F-68D6-4ACC-B8BA-A142D02AD02C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -262,9 +262,18 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
       <right/>
       <top/>
       <bottom/>
@@ -274,13 +283,27 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -294,32 +317,32 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{EE9D6C2C-84DA-46ED-AFC9-95554E0C2B97}" name="Table1" displayName="Table1" ref="A1:W51" totalsRowShown="0">
-  <autoFilter ref="A1:W51" xr:uid="{EE9D6C2C-84DA-46ED-AFC9-95554E0C2B97}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{21DA4E18-08EC-4E02-B52A-7736D1961E75}" name="Table1" displayName="Table1" ref="A1:W51" totalsRowShown="0">
+  <autoFilter ref="A1:W51" xr:uid="{21DA4E18-08EC-4E02-B52A-7736D1961E75}"/>
   <tableColumns count="23">
-    <tableColumn id="1" xr3:uid="{9C6AEF5E-C0E1-4A78-9E5B-3889D1389E27}" name="Genus"/>
-    <tableColumn id="2" xr3:uid="{DD1458EC-D092-4D70-B4BB-4E8C70F88A38}" name="Total_occ"/>
-    <tableColumn id="3" xr3:uid="{C0A8BCE4-9E5E-4B3A-B2EF-2B8D52EF1B0B}" name="Total_occ_with_duplicates"/>
-    <tableColumn id="4" xr3:uid="{067DAF4A-6C5D-41FE-9D58-90707B0F628C}" name="Afrotropics"/>
-    <tableColumn id="5" xr3:uid="{842856DB-8DB1-4F0C-9374-A29068763CB7}" name="Malagasy"/>
-    <tableColumn id="6" xr3:uid="{DD7FB45C-C1AE-47C7-AA4C-C4446D0ABB04}" name="Indomalaya"/>
-    <tableColumn id="7" xr3:uid="{10A07F25-F93F-4460-91AE-365854A8E631}" name="Australasia"/>
-    <tableColumn id="8" xr3:uid="{F2C25E7D-58BB-45A1-BA30-56A73906E652}" name="Neotropics"/>
-    <tableColumn id="9" xr3:uid="{2C4568AD-666F-4E41-86A2-3D6A2D9CCF9B}" name="Western Palearctic"/>
-    <tableColumn id="10" xr3:uid="{4B2D187A-94F7-4C6F-AA04-AF462FFF56D0}" name="Eastern Palearctic"/>
-    <tableColumn id="11" xr3:uid="{E88BD015-6CD3-4D6D-BADB-EB7C7BF66D8B}" name="Nearctic"/>
-    <tableColumn id="12" xr3:uid="{C6567EEA-DE64-40EE-88D8-9FA8C28BA1B4}" name="Palearctic"/>
-    <tableColumn id="13" xr3:uid="{73EAF91C-E3E1-498F-A108-077E1B35197D}" name="Afrotropics_Malagasy"/>
-    <tableColumn id="14" xr3:uid="{5A204F16-9DD3-447B-89B9-0D7A3F8604CB}" name="Afrotropics_duplicates"/>
-    <tableColumn id="15" xr3:uid="{3BC83444-D4D3-4048-82A0-6457049D055D}" name="Malagasy_duplicates"/>
-    <tableColumn id="16" xr3:uid="{2C773334-4FF1-4ADD-B55B-5A0712F8A8C8}" name="Indomalaya_duplicates"/>
-    <tableColumn id="17" xr3:uid="{376C441A-7125-4246-AB5E-EE0ADF490E12}" name="Australasia_duplicates"/>
-    <tableColumn id="18" xr3:uid="{992AADD5-29E2-426A-A999-BD325F124920}" name="Neotropics_duplicates"/>
-    <tableColumn id="19" xr3:uid="{1A8A1452-7871-4E2A-B5A7-9730402EAA73}" name="Western Palearctic_duplicates"/>
-    <tableColumn id="20" xr3:uid="{5809891D-90FE-48FE-9079-9D13990D2D03}" name="Eastern Palearctic_duplicates"/>
-    <tableColumn id="21" xr3:uid="{B24E0D3A-292D-466B-8952-E71BFBBC8FA4}" name="Nearctic_duplicates"/>
-    <tableColumn id="22" xr3:uid="{176312F7-7EF2-41FA-81CF-C37C90B25F76}" name="Palearctic_duplicates"/>
-    <tableColumn id="23" xr3:uid="{0D414638-4D43-4F56-98AA-31985FDB36D5}" name="Afrotropics_Malagasy_duplicates"/>
+    <tableColumn id="1" xr3:uid="{F0A69434-0C1F-42B6-A85E-9526BE569E32}" name="Genus"/>
+    <tableColumn id="2" xr3:uid="{F0D89E0E-6751-4977-917C-9258A3635D5C}" name="Total_occ"/>
+    <tableColumn id="3" xr3:uid="{C35ED9DB-1856-4214-B527-EB02E0A2EC9F}" name="Total_occ_with_duplicates"/>
+    <tableColumn id="4" xr3:uid="{904860E9-7B9F-422F-A3FB-CE27A824B467}" name="Afrotropics"/>
+    <tableColumn id="5" xr3:uid="{258BAA1D-5C7B-4802-8BAC-2E031F99C248}" name="Malagasy"/>
+    <tableColumn id="6" xr3:uid="{6DFBAF6A-8E89-463B-81BB-F6393B1F3705}" name="Indomalaya"/>
+    <tableColumn id="7" xr3:uid="{EA0C6A03-90E6-4C8B-AF81-58E206D3FF42}" name="Australasia"/>
+    <tableColumn id="8" xr3:uid="{264D019D-509D-4F31-97B0-E75064CB9A5B}" name="Neotropics"/>
+    <tableColumn id="9" xr3:uid="{33151CD4-BF58-4447-96AD-9FD4C7BCDC67}" name="Western Palearctic"/>
+    <tableColumn id="10" xr3:uid="{EC783EC9-6F7A-497F-BE04-85F7641FFEC1}" name="Eastern Palearctic"/>
+    <tableColumn id="11" xr3:uid="{CEFA8714-D460-4187-A59D-67105D2650C1}" name="Nearctic"/>
+    <tableColumn id="12" xr3:uid="{5AEA6585-DE26-4A6F-BF81-1DF7444D52EC}" name="Palearctic"/>
+    <tableColumn id="13" xr3:uid="{AE7A391A-8B2C-4B4B-8D13-B9D6CAAA8D80}" name="Afrotropics_Malagasy"/>
+    <tableColumn id="14" xr3:uid="{8DFB1E4D-881F-43BF-98DD-9B3C8CBD91D3}" name="Afrotropics_duplicates" dataDxfId="0"/>
+    <tableColumn id="15" xr3:uid="{58135FE9-1904-4F1E-BAE2-35FED56AAF51}" name="Malagasy_duplicates"/>
+    <tableColumn id="16" xr3:uid="{8182C32D-52E1-404F-9D51-C0D4559B2B22}" name="Indomalaya_duplicates"/>
+    <tableColumn id="17" xr3:uid="{3F7457B1-0F11-4E4B-94AD-C69DC18BD751}" name="Australasia_duplicates"/>
+    <tableColumn id="18" xr3:uid="{7B004C27-6F33-400F-8A73-C3DCD29B72A0}" name="Neotropics_duplicates"/>
+    <tableColumn id="19" xr3:uid="{91C92EC4-CB54-4197-9467-D8D92F11C8EE}" name="Western Palearctic_duplicates"/>
+    <tableColumn id="20" xr3:uid="{1676C85F-C659-4C06-96D7-033C8C90220A}" name="Eastern Palearctic_duplicates"/>
+    <tableColumn id="21" xr3:uid="{A37C946D-10EA-4E4E-8B29-0C9AA58AC101}" name="Nearctic_duplicates"/>
+    <tableColumn id="22" xr3:uid="{739D597E-A0F6-405A-A41E-431B3E4C793D}" name="Palearctic_duplicates"/>
+    <tableColumn id="23" xr3:uid="{0C1752A9-17A5-4E35-92C3-28A5894D381C}" name="Afrotropics_Malagasy_duplicates"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -606,9 +629,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D55" sqref="D55"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -673,7 +695,7 @@
       <c r="M1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
       <c r="O1" t="s">
@@ -709,70 +731,70 @@
         <v>23</v>
       </c>
       <c r="B2">
-        <v>3315</v>
+        <v>3291</v>
       </c>
       <c r="C2">
-        <v>14291</v>
+        <v>14235</v>
       </c>
       <c r="D2">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="E2">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="F2">
-        <v>315</v>
+        <v>326</v>
       </c>
       <c r="G2">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="H2">
-        <v>1426</v>
+        <v>1424</v>
       </c>
       <c r="I2">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="J2">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="K2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L2">
-        <v>77</v>
+        <v>54</v>
       </c>
       <c r="M2">
-        <v>1035</v>
-      </c>
-      <c r="N2">
-        <v>1723</v>
+        <v>1032</v>
+      </c>
+      <c r="N2" s="1">
+        <v>1722</v>
       </c>
       <c r="O2">
-        <v>3675</v>
+        <v>3673</v>
       </c>
       <c r="P2">
-        <v>1161</v>
+        <v>1159</v>
       </c>
       <c r="Q2">
-        <v>1706</v>
+        <v>1696</v>
       </c>
       <c r="R2">
-        <v>5799</v>
+        <v>5797</v>
       </c>
       <c r="S2">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="T2">
-        <v>61</v>
+        <v>31</v>
       </c>
       <c r="U2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V2">
-        <v>226</v>
+        <v>188</v>
       </c>
       <c r="W2">
-        <v>5398</v>
+        <v>5395</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
@@ -815,7 +837,7 @@
       <c r="M3">
         <v>18</v>
       </c>
-      <c r="N3">
+      <c r="N3" s="1">
         <v>68</v>
       </c>
       <c r="O3">
@@ -886,7 +908,7 @@
       <c r="M4">
         <v>0</v>
       </c>
-      <c r="N4">
+      <c r="N4" s="1">
         <v>0</v>
       </c>
       <c r="O4">
@@ -922,10 +944,10 @@
         <v>26</v>
       </c>
       <c r="B5">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C5">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -940,7 +962,7 @@
         <v>0</v>
       </c>
       <c r="H5">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="I5">
         <v>0</v>
@@ -949,7 +971,7 @@
         <v>0</v>
       </c>
       <c r="K5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L5">
         <v>0</v>
@@ -957,7 +979,7 @@
       <c r="M5">
         <v>0</v>
       </c>
-      <c r="N5">
+      <c r="N5" s="1">
         <v>0</v>
       </c>
       <c r="O5">
@@ -970,7 +992,7 @@
         <v>0</v>
       </c>
       <c r="R5">
-        <v>472</v>
+        <v>476</v>
       </c>
       <c r="S5">
         <v>0</v>
@@ -979,7 +1001,7 @@
         <v>0</v>
       </c>
       <c r="U5">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="V5">
         <v>0</v>
@@ -1028,7 +1050,7 @@
       <c r="M6">
         <v>2</v>
       </c>
-      <c r="N6">
+      <c r="N6" s="1">
         <v>23</v>
       </c>
       <c r="O6">
@@ -1064,10 +1086,10 @@
         <v>28</v>
       </c>
       <c r="B7">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="C7">
-        <v>5697</v>
+        <v>5696</v>
       </c>
       <c r="D7">
         <v>693</v>
@@ -1076,7 +1098,7 @@
         <v>533</v>
       </c>
       <c r="F7">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="G7">
         <v>0</v>
@@ -1088,25 +1110,25 @@
         <v>0</v>
       </c>
       <c r="J7">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K7">
         <v>0</v>
       </c>
       <c r="L7">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="M7">
         <v>1226</v>
       </c>
-      <c r="N7">
+      <c r="N7" s="1">
         <v>2180</v>
       </c>
       <c r="O7">
         <v>3239</v>
       </c>
       <c r="P7">
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="Q7">
         <v>0</v>
@@ -1118,13 +1140,13 @@
         <v>0</v>
       </c>
       <c r="T7">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="U7">
         <v>0</v>
       </c>
       <c r="V7">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="W7">
         <v>5419</v>
@@ -1135,10 +1157,10 @@
         <v>29</v>
       </c>
       <c r="B8">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="C8">
-        <v>3453</v>
+        <v>3452</v>
       </c>
       <c r="D8">
         <v>175</v>
@@ -1147,7 +1169,7 @@
         <v>0</v>
       </c>
       <c r="F8">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="G8">
         <v>114</v>
@@ -1159,25 +1181,25 @@
         <v>0</v>
       </c>
       <c r="J8">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="K8">
         <v>0</v>
       </c>
       <c r="L8">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="M8">
         <v>175</v>
       </c>
-      <c r="N8">
+      <c r="N8" s="1">
         <v>670</v>
       </c>
       <c r="O8">
         <v>0</v>
       </c>
       <c r="P8">
-        <v>1244</v>
+        <v>1247</v>
       </c>
       <c r="Q8">
         <v>604</v>
@@ -1189,13 +1211,13 @@
         <v>0</v>
       </c>
       <c r="T8">
-        <v>935</v>
+        <v>931</v>
       </c>
       <c r="U8">
         <v>0</v>
       </c>
       <c r="V8">
-        <v>935</v>
+        <v>931</v>
       </c>
       <c r="W8">
         <v>670</v>
@@ -1241,7 +1263,7 @@
       <c r="M9">
         <v>0</v>
       </c>
-      <c r="N9">
+      <c r="N9" s="1">
         <v>0</v>
       </c>
       <c r="O9">
@@ -1277,13 +1299,13 @@
         <v>31</v>
       </c>
       <c r="B10">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C10">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="D10">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -1310,10 +1332,10 @@
         <v>0</v>
       </c>
       <c r="M10">
-        <v>119</v>
-      </c>
-      <c r="N10">
-        <v>354</v>
+        <v>118</v>
+      </c>
+      <c r="N10" s="1">
+        <v>353</v>
       </c>
       <c r="O10">
         <v>0</v>
@@ -1340,7 +1362,7 @@
         <v>0</v>
       </c>
       <c r="W10">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
@@ -1383,7 +1405,7 @@
       <c r="M11">
         <v>0</v>
       </c>
-      <c r="N11">
+      <c r="N11" s="1">
         <v>0</v>
       </c>
       <c r="O11">
@@ -1419,10 +1441,10 @@
         <v>33</v>
       </c>
       <c r="B12">
-        <v>590</v>
+        <v>581</v>
       </c>
       <c r="C12">
-        <v>2433</v>
+        <v>2413</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -1431,13 +1453,13 @@
         <v>0</v>
       </c>
       <c r="F12">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G12">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="H12">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="I12">
         <v>72</v>
@@ -1446,7 +1468,7 @@
         <v>92</v>
       </c>
       <c r="K12">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="L12">
         <v>164</v>
@@ -1454,20 +1476,20 @@
       <c r="M12">
         <v>0</v>
       </c>
-      <c r="N12">
+      <c r="N12" s="1">
         <v>0</v>
       </c>
       <c r="O12">
         <v>0</v>
       </c>
       <c r="P12">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="Q12">
-        <v>450</v>
+        <v>432</v>
       </c>
       <c r="R12">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="S12">
         <v>220</v>
@@ -1476,7 +1498,7 @@
         <v>468</v>
       </c>
       <c r="U12">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="V12">
         <v>688</v>
@@ -1525,7 +1547,7 @@
       <c r="M13">
         <v>0</v>
       </c>
-      <c r="N13">
+      <c r="N13" s="1">
         <v>0</v>
       </c>
       <c r="O13">
@@ -1596,7 +1618,7 @@
       <c r="M14">
         <v>0</v>
       </c>
-      <c r="N14">
+      <c r="N14" s="1">
         <v>0</v>
       </c>
       <c r="O14">
@@ -1667,7 +1689,7 @@
       <c r="M15">
         <v>7</v>
       </c>
-      <c r="N15">
+      <c r="N15" s="1">
         <v>17</v>
       </c>
       <c r="O15">
@@ -1703,10 +1725,10 @@
         <v>37</v>
       </c>
       <c r="B16">
-        <v>611</v>
+        <v>604</v>
       </c>
       <c r="C16">
-        <v>1855</v>
+        <v>1846</v>
       </c>
       <c r="D16">
         <v>0</v>
@@ -1718,7 +1740,7 @@
         <v>193</v>
       </c>
       <c r="G16">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="H16">
         <v>0</v>
@@ -1727,18 +1749,18 @@
         <v>0</v>
       </c>
       <c r="J16">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="K16">
         <v>0</v>
       </c>
       <c r="L16">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="M16">
         <v>0</v>
       </c>
-      <c r="N16">
+      <c r="N16" s="1">
         <v>0</v>
       </c>
       <c r="O16">
@@ -1748,7 +1770,7 @@
         <v>950</v>
       </c>
       <c r="Q16">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="R16">
         <v>0</v>
@@ -1757,13 +1779,13 @@
         <v>0</v>
       </c>
       <c r="T16">
-        <v>685</v>
+        <v>680</v>
       </c>
       <c r="U16">
         <v>0</v>
       </c>
       <c r="V16">
-        <v>685</v>
+        <v>680</v>
       </c>
       <c r="W16">
         <v>0</v>
@@ -1774,10 +1796,10 @@
         <v>38</v>
       </c>
       <c r="B17">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C17">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="D17">
         <v>0</v>
@@ -1786,7 +1808,7 @@
         <v>0</v>
       </c>
       <c r="F17">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G17">
         <v>0</v>
@@ -1809,14 +1831,14 @@
       <c r="M17">
         <v>0</v>
       </c>
-      <c r="N17">
+      <c r="N17" s="1">
         <v>0</v>
       </c>
       <c r="O17">
         <v>0</v>
       </c>
       <c r="P17">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="Q17">
         <v>0</v>
@@ -1845,13 +1867,13 @@
         <v>39</v>
       </c>
       <c r="B18">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="C18">
-        <v>1233</v>
+        <v>1221</v>
       </c>
       <c r="D18">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E18">
         <v>85</v>
@@ -1860,7 +1882,7 @@
         <v>30</v>
       </c>
       <c r="G18">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H18">
         <v>0</v>
@@ -1869,18 +1891,18 @@
         <v>0</v>
       </c>
       <c r="J18">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="K18">
         <v>0</v>
       </c>
       <c r="L18">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="M18">
-        <v>266</v>
-      </c>
-      <c r="N18">
+        <v>264</v>
+      </c>
+      <c r="N18" s="1">
         <v>502</v>
       </c>
       <c r="O18">
@@ -1890,7 +1912,7 @@
         <v>139</v>
       </c>
       <c r="Q18">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="R18">
         <v>0</v>
@@ -1951,7 +1973,7 @@
       <c r="M19">
         <v>2</v>
       </c>
-      <c r="N19">
+      <c r="N19" s="1">
         <v>5</v>
       </c>
       <c r="O19">
@@ -2022,7 +2044,7 @@
       <c r="M20">
         <v>45</v>
       </c>
-      <c r="N20">
+      <c r="N20" s="1">
         <v>221</v>
       </c>
       <c r="O20">
@@ -2093,7 +2115,7 @@
       <c r="M21">
         <v>77</v>
       </c>
-      <c r="N21">
+      <c r="N21" s="1">
         <v>176</v>
       </c>
       <c r="O21">
@@ -2141,7 +2163,7 @@
         <v>0</v>
       </c>
       <c r="F22">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="G22">
         <v>0</v>
@@ -2153,25 +2175,25 @@
         <v>0</v>
       </c>
       <c r="J22">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="K22">
         <v>0</v>
       </c>
       <c r="L22">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="M22">
         <v>0</v>
       </c>
-      <c r="N22">
+      <c r="N22" s="1">
         <v>0</v>
       </c>
       <c r="O22">
         <v>0</v>
       </c>
       <c r="P22">
-        <v>252</v>
+        <v>263</v>
       </c>
       <c r="Q22">
         <v>0</v>
@@ -2183,13 +2205,13 @@
         <v>0</v>
       </c>
       <c r="T22">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="U22">
         <v>0</v>
       </c>
       <c r="V22">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="W22">
         <v>0</v>
@@ -2200,70 +2222,70 @@
         <v>44</v>
       </c>
       <c r="B23">
-        <v>4656</v>
+        <v>3407</v>
       </c>
       <c r="C23">
-        <v>20343</v>
+        <v>15308</v>
       </c>
       <c r="D23">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="E23">
         <v>319</v>
       </c>
       <c r="F23">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="G23">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="H23">
-        <v>1517</v>
+        <v>1308</v>
       </c>
       <c r="I23">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="J23">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="K23">
-        <v>1149</v>
+        <v>122</v>
       </c>
       <c r="L23">
-        <v>451</v>
+        <v>446</v>
       </c>
       <c r="M23">
-        <v>1026</v>
-      </c>
-      <c r="N23">
-        <v>2446</v>
+        <v>1025</v>
+      </c>
+      <c r="N23" s="1">
+        <v>2448</v>
       </c>
       <c r="O23">
         <v>1043</v>
       </c>
       <c r="P23">
-        <v>691</v>
+        <v>678</v>
       </c>
       <c r="Q23">
-        <v>1250</v>
+        <v>1229</v>
       </c>
       <c r="R23">
-        <v>8720</v>
+        <v>7764</v>
       </c>
       <c r="S23">
-        <v>1066</v>
+        <v>1061</v>
       </c>
       <c r="T23">
-        <v>676</v>
+        <v>671</v>
       </c>
       <c r="U23">
-        <v>4451</v>
+        <v>414</v>
       </c>
       <c r="V23">
-        <v>1742</v>
+        <v>1732</v>
       </c>
       <c r="W23">
-        <v>3489</v>
+        <v>3491</v>
       </c>
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.25">
@@ -2306,7 +2328,7 @@
       <c r="M24">
         <v>0</v>
       </c>
-      <c r="N24">
+      <c r="N24" s="1">
         <v>0</v>
       </c>
       <c r="O24">
@@ -2377,7 +2399,7 @@
       <c r="M25">
         <v>0</v>
       </c>
-      <c r="N25">
+      <c r="N25" s="1">
         <v>0</v>
       </c>
       <c r="O25">
@@ -2413,70 +2435,70 @@
         <v>47</v>
       </c>
       <c r="B26">
-        <v>3214</v>
+        <v>3199</v>
       </c>
       <c r="C26">
-        <v>12176</v>
+        <v>12160</v>
       </c>
       <c r="D26">
-        <v>597</v>
+        <v>603</v>
       </c>
       <c r="E26">
         <v>554</v>
       </c>
       <c r="F26">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="G26">
         <v>330</v>
       </c>
       <c r="H26">
-        <v>912</v>
+        <v>909</v>
       </c>
       <c r="I26">
         <v>3</v>
       </c>
       <c r="J26">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="K26">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="L26">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="M26">
-        <v>1151</v>
-      </c>
-      <c r="N26">
-        <v>1790</v>
+        <v>1157</v>
+      </c>
+      <c r="N26" s="1">
+        <v>1800</v>
       </c>
       <c r="O26">
         <v>2986</v>
       </c>
       <c r="P26">
-        <v>2208</v>
+        <v>2213</v>
       </c>
       <c r="Q26">
         <v>1090</v>
       </c>
       <c r="R26">
-        <v>2584</v>
+        <v>2581</v>
       </c>
       <c r="S26">
         <v>4</v>
       </c>
       <c r="T26">
-        <v>59</v>
+        <v>38</v>
       </c>
       <c r="U26">
-        <v>1455</v>
+        <v>1448</v>
       </c>
       <c r="V26">
-        <v>63</v>
+        <v>42</v>
       </c>
       <c r="W26">
-        <v>4776</v>
+        <v>4786</v>
       </c>
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.25">
@@ -2519,7 +2541,7 @@
       <c r="M27">
         <v>61</v>
       </c>
-      <c r="N27">
+      <c r="N27" s="1">
         <v>171</v>
       </c>
       <c r="O27">
@@ -2590,7 +2612,7 @@
       <c r="M28">
         <v>0</v>
       </c>
-      <c r="N28">
+      <c r="N28" s="1">
         <v>0</v>
       </c>
       <c r="O28">
@@ -2661,7 +2683,7 @@
       <c r="M29">
         <v>184</v>
       </c>
-      <c r="N29">
+      <c r="N29" s="1">
         <v>595</v>
       </c>
       <c r="O29">
@@ -2697,22 +2719,22 @@
         <v>51</v>
       </c>
       <c r="B30">
-        <v>695</v>
+        <v>675</v>
       </c>
       <c r="C30">
-        <v>2438</v>
+        <v>2325</v>
       </c>
       <c r="D30">
         <v>356</v>
       </c>
       <c r="E30">
-        <v>236</v>
+        <v>221</v>
       </c>
       <c r="F30">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G30">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="H30">
         <v>0</v>
@@ -2730,19 +2752,19 @@
         <v>4</v>
       </c>
       <c r="M30">
-        <v>592</v>
-      </c>
-      <c r="N30">
+        <v>577</v>
+      </c>
+      <c r="N30" s="1">
         <v>1153</v>
       </c>
       <c r="O30">
-        <v>1018</v>
+        <v>912</v>
       </c>
       <c r="P30">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="Q30">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="R30">
         <v>0</v>
@@ -2760,7 +2782,7 @@
         <v>18</v>
       </c>
       <c r="W30">
-        <v>2171</v>
+        <v>2065</v>
       </c>
     </row>
     <row r="31" spans="1:23" x14ac:dyDescent="0.25">
@@ -2768,10 +2790,10 @@
         <v>52</v>
       </c>
       <c r="B31">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C31">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="D31">
         <v>0</v>
@@ -2780,7 +2802,7 @@
         <v>0</v>
       </c>
       <c r="F31">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G31">
         <v>130</v>
@@ -2803,14 +2825,14 @@
       <c r="M31">
         <v>0</v>
       </c>
-      <c r="N31">
+      <c r="N31" s="1">
         <v>0</v>
       </c>
       <c r="O31">
         <v>0</v>
       </c>
       <c r="P31">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="Q31">
         <v>412</v>
@@ -2839,10 +2861,10 @@
         <v>53</v>
       </c>
       <c r="B32">
-        <v>4154</v>
+        <v>4152</v>
       </c>
       <c r="C32">
-        <v>13958</v>
+        <v>13956</v>
       </c>
       <c r="D32">
         <v>0</v>
@@ -2857,7 +2879,7 @@
         <v>0</v>
       </c>
       <c r="H32">
-        <v>3999</v>
+        <v>4010</v>
       </c>
       <c r="I32">
         <v>0</v>
@@ -2866,7 +2888,7 @@
         <v>0</v>
       </c>
       <c r="K32">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="L32">
         <v>0</v>
@@ -2874,7 +2896,7 @@
       <c r="M32">
         <v>0</v>
       </c>
-      <c r="N32">
+      <c r="N32" s="1">
         <v>0</v>
       </c>
       <c r="O32">
@@ -2887,7 +2909,7 @@
         <v>0</v>
       </c>
       <c r="R32">
-        <v>13373</v>
+        <v>13405</v>
       </c>
       <c r="S32">
         <v>0</v>
@@ -2896,7 +2918,7 @@
         <v>0</v>
       </c>
       <c r="U32">
-        <v>585</v>
+        <v>551</v>
       </c>
       <c r="V32">
         <v>0</v>
@@ -2910,70 +2932,70 @@
         <v>54</v>
       </c>
       <c r="B33">
-        <v>5326</v>
+        <v>5208</v>
       </c>
       <c r="C33">
-        <v>20731</v>
+        <v>20246</v>
       </c>
       <c r="D33">
         <v>286</v>
       </c>
       <c r="E33">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F33">
-        <v>328</v>
+        <v>319</v>
       </c>
       <c r="G33">
-        <v>765</v>
+        <v>760</v>
       </c>
       <c r="H33">
-        <v>3070</v>
+        <v>3014</v>
       </c>
       <c r="I33">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J33">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K33">
-        <v>742</v>
+        <v>701</v>
       </c>
       <c r="L33">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="M33">
-        <v>395</v>
-      </c>
-      <c r="N33">
-        <v>1424</v>
+        <v>393</v>
+      </c>
+      <c r="N33" s="1">
+        <v>1427</v>
       </c>
       <c r="O33">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="P33">
-        <v>1308</v>
+        <v>1285</v>
       </c>
       <c r="Q33">
-        <v>2623</v>
+        <v>2604</v>
       </c>
       <c r="R33">
-        <v>11762</v>
+        <v>11542</v>
       </c>
       <c r="S33">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="T33">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="U33">
-        <v>2791</v>
+        <v>2576</v>
       </c>
       <c r="V33">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="W33">
-        <v>2134</v>
+        <v>2135</v>
       </c>
     </row>
     <row r="34" spans="1:23" x14ac:dyDescent="0.25">
@@ -2981,10 +3003,10 @@
         <v>55</v>
       </c>
       <c r="B34">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C34">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="D34">
         <v>0</v>
@@ -2996,7 +3018,7 @@
         <v>164</v>
       </c>
       <c r="G34">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H34">
         <v>0</v>
@@ -3016,7 +3038,7 @@
       <c r="M34">
         <v>0</v>
       </c>
-      <c r="N34">
+      <c r="N34" s="1">
         <v>0</v>
       </c>
       <c r="O34">
@@ -3026,7 +3048,7 @@
         <v>569</v>
       </c>
       <c r="Q34">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="R34">
         <v>0</v>
@@ -3087,7 +3109,7 @@
       <c r="M35">
         <v>106</v>
       </c>
-      <c r="N35">
+      <c r="N35" s="1">
         <v>218</v>
       </c>
       <c r="O35">
@@ -3123,10 +3145,10 @@
         <v>57</v>
       </c>
       <c r="B36">
-        <v>1982</v>
+        <v>1980</v>
       </c>
       <c r="C36">
-        <v>8319</v>
+        <v>8317</v>
       </c>
       <c r="D36">
         <v>0</v>
@@ -3135,7 +3157,7 @@
         <v>1</v>
       </c>
       <c r="F36">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G36">
         <v>1</v>
@@ -3150,7 +3172,7 @@
         <v>0</v>
       </c>
       <c r="K36">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="L36">
         <v>0</v>
@@ -3158,14 +3180,14 @@
       <c r="M36">
         <v>1</v>
       </c>
-      <c r="N36">
+      <c r="N36" s="1">
         <v>0</v>
       </c>
       <c r="O36">
         <v>3</v>
       </c>
       <c r="P36">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="Q36">
         <v>4</v>
@@ -3180,7 +3202,7 @@
         <v>0</v>
       </c>
       <c r="U36">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="V36">
         <v>0</v>
@@ -3229,7 +3251,7 @@
       <c r="M37">
         <v>241</v>
       </c>
-      <c r="N37">
+      <c r="N37" s="1">
         <v>933</v>
       </c>
       <c r="O37">
@@ -3265,16 +3287,16 @@
         <v>59</v>
       </c>
       <c r="B38">
-        <v>80</v>
+        <v>56</v>
       </c>
       <c r="C38">
-        <v>268</v>
+        <v>199</v>
       </c>
       <c r="D38">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E38">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="F38">
         <v>29</v>
@@ -3286,7 +3308,7 @@
         <v>0</v>
       </c>
       <c r="I38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J38">
         <v>0</v>
@@ -3295,16 +3317,16 @@
         <v>0</v>
       </c>
       <c r="L38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M38">
-        <v>36</v>
-      </c>
-      <c r="N38">
-        <v>72</v>
+        <v>13</v>
+      </c>
+      <c r="N38" s="1">
+        <v>58</v>
       </c>
       <c r="O38">
-        <v>53</v>
+        <v>0</v>
       </c>
       <c r="P38">
         <v>110</v>
@@ -3316,7 +3338,7 @@
         <v>0</v>
       </c>
       <c r="S38">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T38">
         <v>0</v>
@@ -3325,10 +3347,10 @@
         <v>0</v>
       </c>
       <c r="V38">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="W38">
-        <v>125</v>
+        <v>58</v>
       </c>
     </row>
     <row r="39" spans="1:23" x14ac:dyDescent="0.25">
@@ -3371,7 +3393,7 @@
       <c r="M39">
         <v>129</v>
       </c>
-      <c r="N39">
+      <c r="N39" s="1">
         <v>646</v>
       </c>
       <c r="O39">
@@ -3407,70 +3429,70 @@
         <v>61</v>
       </c>
       <c r="B40">
-        <v>1465</v>
+        <v>1463</v>
       </c>
       <c r="C40">
-        <v>5044</v>
+        <v>5038</v>
       </c>
       <c r="D40">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="E40">
         <v>295</v>
       </c>
       <c r="F40">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="G40">
         <v>206</v>
       </c>
       <c r="H40">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="I40">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J40">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="K40">
         <v>36</v>
       </c>
       <c r="L40">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="M40">
-        <v>634</v>
-      </c>
-      <c r="N40">
-        <v>1225</v>
+        <v>633</v>
+      </c>
+      <c r="N40" s="1">
+        <v>1224</v>
       </c>
       <c r="O40">
         <v>1173</v>
       </c>
       <c r="P40">
-        <v>377</v>
+        <v>383</v>
       </c>
       <c r="Q40">
         <v>495</v>
       </c>
       <c r="R40">
-        <v>1689</v>
+        <v>1690</v>
       </c>
       <c r="S40">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="T40">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="U40">
         <v>50</v>
       </c>
       <c r="V40">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="W40">
-        <v>2398</v>
+        <v>2397</v>
       </c>
     </row>
     <row r="41" spans="1:23" x14ac:dyDescent="0.25">
@@ -3513,7 +3535,7 @@
       <c r="M41">
         <v>365</v>
       </c>
-      <c r="N41">
+      <c r="N41" s="1">
         <v>1221</v>
       </c>
       <c r="O41">
@@ -3549,70 +3571,70 @@
         <v>63</v>
       </c>
       <c r="B42">
-        <v>2466</v>
+        <v>2411</v>
       </c>
       <c r="C42">
-        <v>13694</v>
+        <v>13517</v>
       </c>
       <c r="D42">
         <v>0</v>
       </c>
       <c r="E42">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="F42">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="G42">
-        <v>370</v>
+        <v>365</v>
       </c>
       <c r="H42">
-        <v>102</v>
+        <v>78</v>
       </c>
       <c r="I42">
         <v>630</v>
       </c>
       <c r="J42">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="K42">
-        <v>1056</v>
+        <v>1050</v>
       </c>
       <c r="L42">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="M42">
-        <v>18</v>
-      </c>
-      <c r="N42">
+        <v>4</v>
+      </c>
+      <c r="N42" s="1">
         <v>0</v>
       </c>
       <c r="O42">
-        <v>96</v>
+        <v>20</v>
       </c>
       <c r="P42">
-        <v>548</v>
+        <v>538</v>
       </c>
       <c r="Q42">
-        <v>1314</v>
+        <v>1302</v>
       </c>
       <c r="R42">
-        <v>399</v>
+        <v>342</v>
       </c>
       <c r="S42">
         <v>2413</v>
       </c>
       <c r="T42">
-        <v>989</v>
+        <v>982</v>
       </c>
       <c r="U42">
-        <v>7935</v>
+        <v>7920</v>
       </c>
       <c r="V42">
-        <v>3402</v>
+        <v>3395</v>
       </c>
       <c r="W42">
-        <v>96</v>
+        <v>20</v>
       </c>
     </row>
     <row r="43" spans="1:23" x14ac:dyDescent="0.25">
@@ -3655,7 +3677,7 @@
       <c r="M43">
         <v>11</v>
       </c>
-      <c r="N43">
+      <c r="N43" s="1">
         <v>30</v>
       </c>
       <c r="O43">
@@ -3726,7 +3748,7 @@
       <c r="M44">
         <v>58</v>
       </c>
-      <c r="N44">
+      <c r="N44" s="1">
         <v>219</v>
       </c>
       <c r="O44">
@@ -3762,10 +3784,10 @@
         <v>66</v>
       </c>
       <c r="B45">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C45">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="D45">
         <v>0</v>
@@ -3774,10 +3796,10 @@
         <v>0</v>
       </c>
       <c r="F45">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="G45">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H45">
         <v>0</v>
@@ -3786,28 +3808,28 @@
         <v>0</v>
       </c>
       <c r="J45">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="K45">
         <v>0</v>
       </c>
       <c r="L45">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="M45">
         <v>0</v>
       </c>
-      <c r="N45">
+      <c r="N45" s="1">
         <v>0</v>
       </c>
       <c r="O45">
         <v>0</v>
       </c>
       <c r="P45">
-        <v>514</v>
+        <v>521</v>
       </c>
       <c r="Q45">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="R45">
         <v>0</v>
@@ -3816,13 +3838,13 @@
         <v>0</v>
       </c>
       <c r="T45">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="U45">
         <v>0</v>
       </c>
       <c r="V45">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="W45">
         <v>0</v>
@@ -3868,7 +3890,7 @@
       <c r="M46">
         <v>0</v>
       </c>
-      <c r="N46">
+      <c r="N46" s="1">
         <v>0</v>
       </c>
       <c r="O46">
@@ -3904,10 +3926,10 @@
         <v>68</v>
       </c>
       <c r="B47">
-        <v>407</v>
+        <v>284</v>
       </c>
       <c r="C47">
-        <v>1166</v>
+        <v>874</v>
       </c>
       <c r="D47">
         <v>0</v>
@@ -3922,7 +3944,7 @@
         <v>0</v>
       </c>
       <c r="H47">
-        <v>404</v>
+        <v>281</v>
       </c>
       <c r="I47">
         <v>0</v>
@@ -3939,7 +3961,7 @@
       <c r="M47">
         <v>0</v>
       </c>
-      <c r="N47">
+      <c r="N47" s="1">
         <v>0</v>
       </c>
       <c r="O47">
@@ -3952,7 +3974,7 @@
         <v>0</v>
       </c>
       <c r="R47">
-        <v>1152</v>
+        <v>860</v>
       </c>
       <c r="S47">
         <v>0</v>
@@ -4010,7 +4032,7 @@
       <c r="M48">
         <v>0</v>
       </c>
-      <c r="N48">
+      <c r="N48" s="1">
         <v>0</v>
       </c>
       <c r="O48">
@@ -4081,7 +4103,7 @@
       <c r="M49">
         <v>104</v>
       </c>
-      <c r="N49">
+      <c r="N49" s="1">
         <v>273</v>
       </c>
       <c r="O49">
@@ -4152,7 +4174,7 @@
       <c r="M50">
         <v>0</v>
       </c>
-      <c r="N50">
+      <c r="N50" s="1">
         <v>0</v>
       </c>
       <c r="O50">
@@ -4223,7 +4245,7 @@
       <c r="M51">
         <v>0</v>
       </c>
-      <c r="N51">
+      <c r="N51" s="1">
         <v>0</v>
       </c>
       <c r="O51">

</xml_diff>